<commit_message>
se agrega la grafica y se actualiza el requirements porque requeri de unas dependencias para q la chart funcionara
</commit_message>
<xml_diff>
--- a/reservas_viajes_completas.xlsx
+++ b/reservas_viajes_completas.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,14 +16,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +48,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,47 +441,47 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Destino</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Personas</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Fecha Viaje</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Fecha Registro</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Cédula</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Apellido</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Teléfono</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Correo</t>
         </is>
@@ -1005,6 +1024,1742 @@
       <c r="I13" t="inlineStr">
         <is>
           <t>yeyeyeyey@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:01</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>45678</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>pepe</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>lopex</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>11111</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>pepe@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:24</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>545454</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>pepe</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>333</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>pepe@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:41</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>sddd</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>dd@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:43</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>555</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>561</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>ss@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Francia</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:44</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2222</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>22233</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>c@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Italia</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>5</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-03-29</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:46</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>78787</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>fggg</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>ggg@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Italia</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:50</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>1454545</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>98979</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>r@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:51</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>222333</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>t@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>5</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:52</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>4555</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>zz</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>677</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>l@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2025-03-21 02:56</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>98979</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>t@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:01</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>23456</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>4555</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>zz</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>5554</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>a@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:28</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>1454545</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>98979</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>r@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>7</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:28</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>122222</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>22222</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>y@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>5</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2025-03-27</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:29</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>576676</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>567756</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>b@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4" t="n">
+        <v>45737</v>
+      </c>
+      <c r="D33" s="5" t="n">
+        <v>45737.14880532408</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:41</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>1454545</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>98979</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>r@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Italia</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:43</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>1454545</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>98979</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>r@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2025-03-22</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:44</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>22222</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>56767677</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>y@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>5</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:45</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>889</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>99977979</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>i@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>3</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:46</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>070707</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>8687686</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>i@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>3</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:46</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>3333</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>rt</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>rt</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>333333</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>rt@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>3</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:47</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2222223343</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>rruur</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>rr</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>343454345</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>rr@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Francia</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>8</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2025-03-22</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:47</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>645456</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>43545</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>ir@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Francia</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>8</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2025-03-22</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:48</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>3443</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>rr</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>rr</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>5545</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>i@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Francia</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:49</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>343443</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>rr</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>343434343</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>r@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Francia</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:52</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>98979</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>t@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Francia</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>4</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:53</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>4545545</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>mjjjkj</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>jkj</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>4545454545</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>m@mial.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Italia</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:58</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>232313</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>45454545</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>t@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Italia</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>2</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:59</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>34555656</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>jj</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>lool</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>65565656</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>l@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Italia</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>3</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2025-03-21 03:59</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>787878</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>8978897</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>u@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Italia</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>4</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2025-03-21 04:00</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>87878</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>24242454</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>r@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Italia</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>5</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2025-03-21 04:01</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>46676</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>4554343j</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>76657576</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>56@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Francia</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>5</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2025-03-21 04:02</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>787</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>ui</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>7868</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>ui@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Francia</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>4</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2025-03-21 04:02</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>56646456</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>uui</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>ww</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>5464645</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>w@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>1</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2025-03-21 04:03</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>7657665</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>jj</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>io</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>665656</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>i@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>4</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2025-03-29</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2025-03-21 04:07</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>45445</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>zz</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>677</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>ggg@mail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>4</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2025-03-29</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2025-03-21 04:07</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>67676</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>88989</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>y@mail.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se realizan ajustes de titulo y grafico
</commit_message>
<xml_diff>
--- a/reservas_viajes_completas.xlsx
+++ b/reservas_viajes_completas.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2763,6 +2763,456 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2025-03-21 13:33</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>3333</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>gg</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>3333</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>f@gmail.cpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2025-03-21 13:35</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>555554</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>lulu</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>perez</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>p@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Francia</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2025-03-21 13:41</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>lula</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>li</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>lu@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>5</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2025-03-21 13:45</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>juan</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>jun</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>5656</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>jj@gmai.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>10</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2025-03-21 13:51</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>lina</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>marin</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>45545</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>l@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2025-03-21 13:58</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>ff</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>f@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2025-03-21 14:34</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>23423423</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>sfdsfs</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>dsfsdfs</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>234324</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>wfwe@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2025-03-21 14:38</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>s@gmal.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2025-03-22</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2025-03-21 14:44</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>3233333</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>luis</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>lopez</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>333</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>luis@gmai.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2025-03-21 14:54</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>32333444</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>tulio</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>lopez</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>5555555</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>lopez@gmail.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>